<commit_message>
Added phenology figures. removed some column heading errors from data files
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Wagga2008.xlsx
+++ b/Prototypes/Canola/Wagga2008.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF9C289-D81A-47D4-AF9B-3921AEBCB281}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ECB3AD-53AF-4CD0-B414-6C3B3B592B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="24420" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="46">
   <si>
     <t>HAr GAI</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Canola.Stage</t>
+  </si>
+  <si>
+    <t>Canola.Grain.Size</t>
+  </si>
+  <si>
+    <t>Canola.Grain.SizeError</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1DBC07-D785-4055-8068-A40DE3AED641}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AK97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="I91" sqref="I91"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="R121" sqref="R121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,14 +555,14 @@
     <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19.140625" bestFit="1" customWidth="1"/>
@@ -627,7 +634,7 @@
         <v>10</v>
       </c>
       <c r="S1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="T1" t="s">
         <v>15</v>
@@ -666,7 +673,7 @@
         <v>29</v>
       </c>
       <c r="AF1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AG1" t="s">
         <v>31</v>
@@ -684,7 +691,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>C2&amp;B2&amp;"Cv"&amp;D2&amp;"Treat"&amp;E2</f>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -765,7 +772,7 @@
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">C3&amp;B3&amp;"Cv"&amp;D3&amp;"Treat"&amp;E3</f>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -844,7 +851,7 @@
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -925,7 +932,7 @@
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1006,7 +1013,7 @@
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1087,7 +1094,7 @@
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1275,7 +1282,7 @@
         <v>1.5082910959437631E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1342,7 +1349,7 @@
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1415,7 +1422,7 @@
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1496,7 +1503,7 @@
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1577,7 +1584,7 @@
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1658,7 +1665,7 @@
       <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1846,7 +1853,7 @@
         <v>7.3689311541742753E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -1927,7 +1934,7 @@
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2006,7 +2013,7 @@
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2087,7 +2094,7 @@
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2168,7 +2175,7 @@
       <c r="AJ19" s="3"/>
       <c r="AK19" s="3"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2249,7 +2256,7 @@
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2437,7 +2444,7 @@
         <v>2.4262733164717942E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2518,7 +2525,7 @@
       <c r="AJ23" s="3"/>
       <c r="AK23" s="3"/>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2597,7 +2604,7 @@
       <c r="AJ24" s="3"/>
       <c r="AK24" s="3"/>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2678,7 +2685,7 @@
       <c r="AJ25" s="3"/>
       <c r="AK25" s="3"/>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2759,7 +2766,7 @@
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3"/>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2840,7 +2847,7 @@
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -3028,7 +3035,7 @@
         <v>1.6341572459386597E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3109,7 +3116,7 @@
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3188,7 +3195,7 @@
       <c r="AJ31" s="3"/>
       <c r="AK31" s="3"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3269,7 +3276,7 @@
       <c r="AJ32" s="3"/>
       <c r="AK32" s="3"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3350,7 +3357,7 @@
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3431,7 +3438,7 @@
       <c r="AJ34" s="3"/>
       <c r="AK34" s="3"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3619,7 +3626,7 @@
         <v>1.594680804767807E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3686,7 +3693,7 @@
       <c r="AJ37" s="3"/>
       <c r="AK37" s="3"/>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3759,7 +3766,7 @@
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3840,7 +3847,7 @@
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3921,7 +3928,7 @@
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -4002,7 +4009,7 @@
       <c r="AJ41" s="3"/>
       <c r="AK41" s="3"/>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -4190,7 +4197,7 @@
         <v>3.0796328121556358E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4271,7 +4278,7 @@
       <c r="AJ44" s="3"/>
       <c r="AK44" s="3"/>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4350,7 +4357,7 @@
       <c r="AJ45" s="3"/>
       <c r="AK45" s="3"/>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4431,7 +4438,7 @@
       <c r="AJ46" s="3"/>
       <c r="AK46" s="3"/>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4512,7 +4519,7 @@
       <c r="AJ47" s="3"/>
       <c r="AK47" s="3"/>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4593,7 +4600,7 @@
       <c r="AJ48" s="3"/>
       <c r="AK48" s="3"/>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4781,7 +4788,7 @@
         <v>6.8418886233867415E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -4862,7 +4869,7 @@
       <c r="AJ51" s="3"/>
       <c r="AK51" s="3"/>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -4941,7 +4948,7 @@
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3"/>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5022,7 +5029,7 @@
       <c r="AJ53" s="3"/>
       <c r="AK53" s="3"/>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5103,7 +5110,7 @@
       <c r="AJ54" s="3"/>
       <c r="AK54" s="3"/>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5184,7 +5191,7 @@
       <c r="AJ55" s="3"/>
       <c r="AK55" s="3"/>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5372,7 +5379,7 @@
         <v>1.6838512560928193E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5453,7 +5460,7 @@
       <c r="AJ58" s="3"/>
       <c r="AK58" s="3"/>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5532,7 +5539,7 @@
       <c r="AJ59" s="3"/>
       <c r="AK59" s="3"/>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5613,7 +5620,7 @@
       <c r="AJ60" s="3"/>
       <c r="AK60" s="3"/>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5694,7 +5701,7 @@
       <c r="AJ61" s="3"/>
       <c r="AK61" s="3"/>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5775,7 +5782,7 @@
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3"/>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5963,7 +5970,7 @@
         <v>1.8344854302389708E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6030,7 +6037,7 @@
       <c r="AJ65" s="3"/>
       <c r="AK65" s="3"/>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6103,7 +6110,7 @@
       <c r="AJ66" s="3"/>
       <c r="AK66" s="3"/>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" ref="A67:A85" si="2">C67&amp;B67&amp;"Cv"&amp;D67&amp;"Treat"&amp;E67</f>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6184,7 +6191,7 @@
       <c r="AJ67" s="3"/>
       <c r="AK67" s="3"/>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6265,7 +6272,7 @@
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6346,7 +6353,7 @@
       <c r="AJ69" s="3"/>
       <c r="AK69" s="3"/>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6534,7 +6541,7 @@
         <v>1.1817984780042505E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6615,7 +6622,7 @@
       <c r="AJ72" s="3"/>
       <c r="AK72" s="3"/>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6694,7 +6701,7 @@
       <c r="AJ73" s="3"/>
       <c r="AK73" s="3"/>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6775,7 +6782,7 @@
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6856,7 +6863,7 @@
       <c r="AJ75" s="3"/>
       <c r="AK75" s="3"/>
     </row>
-    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6937,7 +6944,7 @@
       <c r="AJ76" s="3"/>
       <c r="AK76" s="3"/>
     </row>
-    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -7125,7 +7132,7 @@
         <v>1.1129064835374528E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7206,7 +7213,7 @@
       <c r="AJ79" s="3"/>
       <c r="AK79" s="3"/>
     </row>
-    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7285,7 +7292,7 @@
       <c r="AJ80" s="3"/>
       <c r="AK80" s="3"/>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7366,7 +7373,7 @@
       <c r="AJ81" s="3"/>
       <c r="AK81" s="3"/>
     </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7447,7 +7454,7 @@
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3"/>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7528,7 +7535,7 @@
       <c r="AJ83" s="3"/>
       <c r="AK83" s="3"/>
     </row>
-    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7993,7 +8000,13 @@
       <c r="P97" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK85" xr:uid="{88E473E4-03DA-403D-83E8-A09F834A928F}"/>
+  <autoFilter ref="A1:AK85" xr:uid="{88E473E4-03DA-403D-83E8-A09F834A928F}">
+    <filterColumn colId="22">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Consistent variable names in Wagga file, decimal place in leaf appearance OCP, extended grainfilling to 700 degdays
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Wagga2008.xlsx
+++ b/Prototypes/Canola/Wagga2008.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ECB3AD-53AF-4CD0-B414-6C3B3B592B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1C385C-4B7B-473D-9176-BB325166F230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="24420" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="3" r:id="rId1"/>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Clock.Today</t>
-  </si>
-  <si>
-    <t>Canola.Cultivar</t>
   </si>
   <si>
     <t>Canola.Leaf.Live.Wt</t>
@@ -161,9 +158,6 @@
     <t>Canola.Pod.WtError</t>
   </si>
   <si>
-    <t>Canola.SowingDate</t>
-  </si>
-  <si>
     <t>Canola.DaysAfterSowing</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>Canola.Grain.SizeError</t>
+  </si>
+  <si>
+    <t>Cv</t>
+  </si>
+  <si>
+    <t>SowingDate</t>
   </si>
 </sst>
 </file>
@@ -535,11 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1DBC07-D785-4055-8068-A40DE3AED641}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AK97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="R121" sqref="R121"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,118 +579,118 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" t="s">
         <v>13</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" t="s">
-        <v>14</v>
       </c>
       <c r="V1" t="s">
         <v>0</v>
       </c>
       <c r="W1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X1" t="s">
         <v>1</v>
       </c>
       <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>C2&amp;B2&amp;"Cv"&amp;D2&amp;"Treat"&amp;E2</f>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -700,7 +699,7 @@
         <v>2008</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -772,7 +771,7 @@
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
     </row>
-    <row r="3" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">C3&amp;B3&amp;"Cv"&amp;D3&amp;"Treat"&amp;E3</f>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -781,7 +780,7 @@
         <v>2008</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -807,7 +806,7 @@
         <v>66</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" s="5">
         <v>187.38749999999999</v>
@@ -851,7 +850,7 @@
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
     </row>
-    <row r="4" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -860,7 +859,7 @@
         <v>2008</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -932,7 +931,7 @@
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
     </row>
-    <row r="5" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -941,7 +940,7 @@
         <v>2008</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -1013,7 +1012,7 @@
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
     </row>
-    <row r="6" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1022,7 +1021,7 @@
         <v>2008</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1094,7 +1093,7 @@
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
     </row>
-    <row r="7" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1103,7 +1102,7 @@
         <v>2008</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1184,7 +1183,7 @@
         <v>2008</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1282,7 +1281,7 @@
         <v>1.5082910959437631E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1291,13 +1290,13 @@
         <v>2008</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9">
         <v>48</v>
@@ -1323,7 +1322,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
@@ -1349,7 +1348,7 @@
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3"/>
     </row>
-    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1358,13 +1357,13 @@
         <v>2008</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10">
         <v>48</v>
@@ -1384,7 +1383,7 @@
         <v>57</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M10" s="5">
         <v>28.410648148148152</v>
@@ -1394,7 +1393,7 @@
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
@@ -1422,7 +1421,7 @@
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
     </row>
-    <row r="11" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1431,13 +1430,13 @@
         <v>2008</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11">
         <v>48</v>
@@ -1503,7 +1502,7 @@
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
     </row>
-    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1512,13 +1511,13 @@
         <v>2008</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12">
         <v>48</v>
@@ -1584,7 +1583,7 @@
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
     </row>
-    <row r="13" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1593,13 +1592,13 @@
         <v>2008</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13">
         <v>48</v>
@@ -1665,7 +1664,7 @@
       <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
     </row>
-    <row r="14" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1674,13 +1673,13 @@
         <v>2008</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14">
         <v>48</v>
@@ -1755,13 +1754,13 @@
         <v>2008</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15">
         <v>48</v>
@@ -1853,7 +1852,7 @@
         <v>7.3689311541742753E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -1862,7 +1861,7 @@
         <v>2008</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -1934,7 +1933,7 @@
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
     </row>
-    <row r="17" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -1943,7 +1942,7 @@
         <v>2008</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -1969,7 +1968,7 @@
         <v>66</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M17" s="5">
         <v>113.0895</v>
@@ -2013,7 +2012,7 @@
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
     </row>
-    <row r="18" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2022,7 +2021,7 @@
         <v>2008</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -2094,7 +2093,7 @@
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
     </row>
-    <row r="19" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2103,7 +2102,7 @@
         <v>2008</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -2175,7 +2174,7 @@
       <c r="AJ19" s="3"/>
       <c r="AK19" s="3"/>
     </row>
-    <row r="20" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2184,7 +2183,7 @@
         <v>2008</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -2256,7 +2255,7 @@
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
     </row>
-    <row r="21" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2265,7 +2264,7 @@
         <v>2008</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -2346,7 +2345,7 @@
         <v>2008</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
@@ -2444,7 +2443,7 @@
         <v>2.4262733164717942E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2453,7 +2452,7 @@
         <v>2008</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -2525,7 +2524,7 @@
       <c r="AJ23" s="3"/>
       <c r="AK23" s="3"/>
     </row>
-    <row r="24" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2534,7 +2533,7 @@
         <v>2008</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -2560,7 +2559,7 @@
         <v>66</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M24" s="5">
         <v>167.26512499999998</v>
@@ -2604,7 +2603,7 @@
       <c r="AJ24" s="3"/>
       <c r="AK24" s="3"/>
     </row>
-    <row r="25" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2613,7 +2612,7 @@
         <v>2008</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -2685,7 +2684,7 @@
       <c r="AJ25" s="3"/>
       <c r="AK25" s="3"/>
     </row>
-    <row r="26" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2694,7 +2693,7 @@
         <v>2008</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -2766,7 +2765,7 @@
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3"/>
     </row>
-    <row r="27" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2775,7 +2774,7 @@
         <v>2008</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -2847,7 +2846,7 @@
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
     </row>
-    <row r="28" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2856,7 +2855,7 @@
         <v>2008</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -2937,7 +2936,7 @@
         <v>2008</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -3035,7 +3034,7 @@
         <v>1.6341572459386597E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3044,10 +3043,10 @@
         <v>2008</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
@@ -3116,7 +3115,7 @@
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
     </row>
-    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3125,10 +3124,10 @@
         <v>2008</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -3151,7 +3150,7 @@
         <v>66</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M31" s="5">
         <v>187.38749999999996</v>
@@ -3195,7 +3194,7 @@
       <c r="AJ31" s="3"/>
       <c r="AK31" s="3"/>
     </row>
-    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3204,10 +3203,10 @@
         <v>2008</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -3276,7 +3275,7 @@
       <c r="AJ32" s="3"/>
       <c r="AK32" s="3"/>
     </row>
-    <row r="33" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3285,10 +3284,10 @@
         <v>2008</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -3357,7 +3356,7 @@
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
     </row>
-    <row r="34" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3366,10 +3365,10 @@
         <v>2008</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -3438,7 +3437,7 @@
       <c r="AJ34" s="3"/>
       <c r="AK34" s="3"/>
     </row>
-    <row r="35" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3447,10 +3446,10 @@
         <v>2008</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
         <v>4</v>
@@ -3528,10 +3527,10 @@
         <v>2008</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
         <v>4</v>
@@ -3626,7 +3625,7 @@
         <v>1.594680804767807E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3635,13 +3634,13 @@
         <v>2008</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F37">
         <v>48</v>
@@ -3667,7 +3666,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
@@ -3693,7 +3692,7 @@
       <c r="AJ37" s="3"/>
       <c r="AK37" s="3"/>
     </row>
-    <row r="38" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3702,13 +3701,13 @@
         <v>2008</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F38">
         <v>48</v>
@@ -3728,7 +3727,7 @@
         <v>57</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M38" s="5">
         <v>22.952546296296294</v>
@@ -3738,7 +3737,7 @@
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
@@ -3766,7 +3765,7 @@
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
     </row>
-    <row r="39" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3775,13 +3774,13 @@
         <v>2008</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F39">
         <v>48</v>
@@ -3847,7 +3846,7 @@
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
     </row>
-    <row r="40" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3856,13 +3855,13 @@
         <v>2008</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F40">
         <v>48</v>
@@ -3928,7 +3927,7 @@
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
     </row>
-    <row r="41" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3937,13 +3936,13 @@
         <v>2008</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F41">
         <v>48</v>
@@ -4009,7 +4008,7 @@
       <c r="AJ41" s="3"/>
       <c r="AK41" s="3"/>
     </row>
-    <row r="42" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -4018,13 +4017,13 @@
         <v>2008</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F42">
         <v>48</v>
@@ -4099,13 +4098,13 @@
         <v>2008</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43">
         <v>48</v>
@@ -4197,7 +4196,7 @@
         <v>3.0796328121556358E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4206,10 +4205,10 @@
         <v>2008</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E44" t="s">
         <v>2</v>
@@ -4278,7 +4277,7 @@
       <c r="AJ44" s="3"/>
       <c r="AK44" s="3"/>
     </row>
-    <row r="45" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4287,10 +4286,10 @@
         <v>2008</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" t="s">
         <v>2</v>
@@ -4313,7 +4312,7 @@
         <v>66</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M45" s="5">
         <v>106.12406249999999</v>
@@ -4357,7 +4356,7 @@
       <c r="AJ45" s="3"/>
       <c r="AK45" s="3"/>
     </row>
-    <row r="46" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4366,10 +4365,10 @@
         <v>2008</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s">
         <v>2</v>
@@ -4438,7 +4437,7 @@
       <c r="AJ46" s="3"/>
       <c r="AK46" s="3"/>
     </row>
-    <row r="47" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4447,10 +4446,10 @@
         <v>2008</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s">
         <v>2</v>
@@ -4519,7 +4518,7 @@
       <c r="AJ47" s="3"/>
       <c r="AK47" s="3"/>
     </row>
-    <row r="48" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4528,10 +4527,10 @@
         <v>2008</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48" t="s">
         <v>2</v>
@@ -4600,7 +4599,7 @@
       <c r="AJ48" s="3"/>
       <c r="AK48" s="3"/>
     </row>
-    <row r="49" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4609,10 +4608,10 @@
         <v>2008</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E49" t="s">
         <v>2</v>
@@ -4690,10 +4689,10 @@
         <v>2008</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E50" t="s">
         <v>2</v>
@@ -4788,7 +4787,7 @@
         <v>6.8418886233867415E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -4797,10 +4796,10 @@
         <v>2008</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51" t="s">
         <v>3</v>
@@ -4869,7 +4868,7 @@
       <c r="AJ51" s="3"/>
       <c r="AK51" s="3"/>
     </row>
-    <row r="52" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -4878,10 +4877,10 @@
         <v>2008</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
@@ -4904,7 +4903,7 @@
         <v>66</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M52" s="5">
         <v>151.0124375</v>
@@ -4948,7 +4947,7 @@
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3"/>
     </row>
-    <row r="53" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -4957,10 +4956,10 @@
         <v>2008</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
         <v>3</v>
@@ -5029,7 +5028,7 @@
       <c r="AJ53" s="3"/>
       <c r="AK53" s="3"/>
     </row>
-    <row r="54" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5038,10 +5037,10 @@
         <v>2008</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E54" t="s">
         <v>3</v>
@@ -5110,7 +5109,7 @@
       <c r="AJ54" s="3"/>
       <c r="AK54" s="3"/>
     </row>
-    <row r="55" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5119,10 +5118,10 @@
         <v>2008</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
@@ -5191,7 +5190,7 @@
       <c r="AJ55" s="3"/>
       <c r="AK55" s="3"/>
     </row>
-    <row r="56" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5200,10 +5199,10 @@
         <v>2008</v>
       </c>
       <c r="C56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56" t="s">
         <v>3</v>
@@ -5281,10 +5280,10 @@
         <v>2008</v>
       </c>
       <c r="C57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s">
         <v>3</v>
@@ -5379,7 +5378,7 @@
         <v>1.6838512560928193E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5388,10 +5387,10 @@
         <v>2008</v>
       </c>
       <c r="C58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E58" t="s">
         <v>4</v>
@@ -5460,7 +5459,7 @@
       <c r="AJ58" s="3"/>
       <c r="AK58" s="3"/>
     </row>
-    <row r="59" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5469,10 +5468,10 @@
         <v>2008</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E59" t="s">
         <v>4</v>
@@ -5495,7 +5494,7 @@
         <v>66</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M59" s="5">
         <v>107.67193750000001</v>
@@ -5539,7 +5538,7 @@
       <c r="AJ59" s="3"/>
       <c r="AK59" s="3"/>
     </row>
-    <row r="60" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5548,10 +5547,10 @@
         <v>2008</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E60" t="s">
         <v>4</v>
@@ -5620,7 +5619,7 @@
       <c r="AJ60" s="3"/>
       <c r="AK60" s="3"/>
     </row>
-    <row r="61" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5629,10 +5628,10 @@
         <v>2008</v>
       </c>
       <c r="C61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E61" t="s">
         <v>4</v>
@@ -5701,7 +5700,7 @@
       <c r="AJ61" s="3"/>
       <c r="AK61" s="3"/>
     </row>
-    <row r="62" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5710,10 +5709,10 @@
         <v>2008</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
@@ -5782,7 +5781,7 @@
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3"/>
     </row>
-    <row r="63" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5791,10 +5790,10 @@
         <v>2008</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E63" t="s">
         <v>4</v>
@@ -5872,10 +5871,10 @@
         <v>2008</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E64" t="s">
         <v>4</v>
@@ -5970,7 +5969,7 @@
         <v>1.8344854302389708E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -5979,13 +5978,13 @@
         <v>2008</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E65" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F65">
         <v>48</v>
@@ -6011,7 +6010,7 @@
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="P65" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q65" s="3"/>
       <c r="R65" s="3"/>
@@ -6037,7 +6036,7 @@
       <c r="AJ65" s="3"/>
       <c r="AK65" s="3"/>
     </row>
-    <row r="66" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6046,13 +6045,13 @@
         <v>2008</v>
       </c>
       <c r="C66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F66">
         <v>48</v>
@@ -6072,7 +6071,7 @@
         <v>57</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M66" s="5">
         <v>16.098611111111111</v>
@@ -6082,7 +6081,7 @@
       </c>
       <c r="O66" s="3"/>
       <c r="P66" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
@@ -6110,7 +6109,7 @@
       <c r="AJ66" s="3"/>
       <c r="AK66" s="3"/>
     </row>
-    <row r="67" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" ref="A67:A85" si="2">C67&amp;B67&amp;"Cv"&amp;D67&amp;"Treat"&amp;E67</f>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6119,13 +6118,13 @@
         <v>2008</v>
       </c>
       <c r="C67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D67" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F67">
         <v>48</v>
@@ -6191,7 +6190,7 @@
       <c r="AJ67" s="3"/>
       <c r="AK67" s="3"/>
     </row>
-    <row r="68" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6200,13 +6199,13 @@
         <v>2008</v>
       </c>
       <c r="C68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F68">
         <v>48</v>
@@ -6272,7 +6271,7 @@
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
     </row>
-    <row r="69" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6281,13 +6280,13 @@
         <v>2008</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F69">
         <v>48</v>
@@ -6353,7 +6352,7 @@
       <c r="AJ69" s="3"/>
       <c r="AK69" s="3"/>
     </row>
-    <row r="70" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6362,13 +6361,13 @@
         <v>2008</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F70">
         <v>48</v>
@@ -6443,13 +6442,13 @@
         <v>2008</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D71" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F71">
         <v>48</v>
@@ -6541,7 +6540,7 @@
         <v>1.1817984780042505E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6550,10 +6549,10 @@
         <v>2008</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E72" t="s">
         <v>2</v>
@@ -6622,7 +6621,7 @@
       <c r="AJ72" s="3"/>
       <c r="AK72" s="3"/>
     </row>
-    <row r="73" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6631,10 +6630,10 @@
         <v>2008</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E73" t="s">
         <v>2</v>
@@ -6657,7 +6656,7 @@
         <v>66</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M73" s="5">
         <v>41.113312499999992</v>
@@ -6701,7 +6700,7 @@
       <c r="AJ73" s="3"/>
       <c r="AK73" s="3"/>
     </row>
-    <row r="74" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6710,10 +6709,10 @@
         <v>2008</v>
       </c>
       <c r="C74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E74" t="s">
         <v>2</v>
@@ -6782,7 +6781,7 @@
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
     </row>
-    <row r="75" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6791,10 +6790,10 @@
         <v>2008</v>
       </c>
       <c r="C75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E75" t="s">
         <v>2</v>
@@ -6863,7 +6862,7 @@
       <c r="AJ75" s="3"/>
       <c r="AK75" s="3"/>
     </row>
-    <row r="76" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6872,10 +6871,10 @@
         <v>2008</v>
       </c>
       <c r="C76" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D76" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E76" t="s">
         <v>2</v>
@@ -6944,7 +6943,7 @@
       <c r="AJ76" s="3"/>
       <c r="AK76" s="3"/>
     </row>
-    <row r="77" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6953,10 +6952,10 @@
         <v>2008</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D77" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E77" t="s">
         <v>2</v>
@@ -7034,10 +7033,10 @@
         <v>2008</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D78" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E78" t="s">
         <v>2</v>
@@ -7132,7 +7131,7 @@
         <v>1.1129064835374528E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7141,10 +7140,10 @@
         <v>2008</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E79" t="s">
         <v>3</v>
@@ -7213,7 +7212,7 @@
       <c r="AJ79" s="3"/>
       <c r="AK79" s="3"/>
     </row>
-    <row r="80" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7222,10 +7221,10 @@
         <v>2008</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D80" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E80" t="s">
         <v>3</v>
@@ -7248,7 +7247,7 @@
         <v>66</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M80" s="5">
         <v>79.810187500000012</v>
@@ -7292,7 +7291,7 @@
       <c r="AJ80" s="3"/>
       <c r="AK80" s="3"/>
     </row>
-    <row r="81" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7301,10 +7300,10 @@
         <v>2008</v>
       </c>
       <c r="C81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E81" t="s">
         <v>3</v>
@@ -7373,7 +7372,7 @@
       <c r="AJ81" s="3"/>
       <c r="AK81" s="3"/>
     </row>
-    <row r="82" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7382,10 +7381,10 @@
         <v>2008</v>
       </c>
       <c r="C82" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E82" t="s">
         <v>3</v>
@@ -7454,7 +7453,7 @@
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3"/>
     </row>
-    <row r="83" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7463,10 +7462,10 @@
         <v>2008</v>
       </c>
       <c r="C83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D83" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E83" t="s">
         <v>3</v>
@@ -7535,7 +7534,7 @@
       <c r="AJ83" s="3"/>
       <c r="AK83" s="3"/>
     </row>
-    <row r="84" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7544,10 +7543,10 @@
         <v>2008</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D84" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E84" t="s">
         <v>3</v>
@@ -7625,10 +7624,10 @@
         <v>2008</v>
       </c>
       <c r="C85" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D85" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E85" t="s">
         <v>3</v>
@@ -8000,13 +7999,7 @@
       <c r="P97" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK85" xr:uid="{88E473E4-03DA-403D-83E8-A09F834A928F}">
-    <filterColumn colId="22">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AK85" xr:uid="{88E473E4-03DA-403D-83E8-A09F834A928F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>